<commit_message>
modify the childnodes counting and simplify the codes
</commit_message>
<xml_diff>
--- a/Practical14/autophagosome.xlsx
+++ b/Practical14/autophagosome.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GO:0000045</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -472,13 +472,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GO:0000421</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GO:0016236</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GO:0016237</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -532,13 +532,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GO:0016240</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GO:0016243</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GO:0030399</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GO:0032258</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -612,13 +612,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GO:0034423</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -632,13 +632,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GO:0044753</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GO:0044754</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -672,13 +672,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GO:0045771</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -692,13 +692,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GO:0045772</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GO:0048102</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GO:0061709</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -752,13 +752,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GO:0061739</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -772,13 +772,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GO:0061753</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -792,13 +792,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GO:0061906</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -812,13 +812,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GO:0061908</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GO:0061909</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -852,13 +852,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GO:0061910</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -872,13 +872,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GO:0097635</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -892,13 +892,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GO:0097636</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -918,7 +918,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GO:0097637</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -932,13 +932,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GO:0098792</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -952,13 +952,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GO:0120095</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -972,13 +972,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GO:1901096</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -992,13 +992,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GO:1901097</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1012,13 +1012,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GO:1901098</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1032,13 +1032,13 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GO:1901245</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1052,13 +1052,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GO:1902902</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1072,13 +1072,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GO:1905037</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GO:1990316</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1112,13 +1112,13 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GO:1990462</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1132,13 +1132,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GO:2000785</t>
+          <t>&lt;built-in function id&gt;</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the nodes-counting part
</commit_message>
<xml_diff>
--- a/Practical14/autophagosome.xlsx
+++ b/Practical14/autophagosome.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0000045</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,7 +478,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0000421</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0016236</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,13 +512,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0016237</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -538,7 +538,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0016240</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0016243</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0030399</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0032258</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -618,7 +618,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0034423</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0044753</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -658,7 +658,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0044754</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -678,7 +678,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0045771</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0045772</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -718,7 +718,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0048102</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061709</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061739</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -778,7 +778,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061753</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -798,7 +798,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061906</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061908</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -838,7 +838,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061909</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -858,7 +858,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0061910</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0097635</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -898,7 +898,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0097636</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -918,7 +918,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0097637</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0098792</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -958,7 +958,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:0120095</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -978,7 +978,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1901096</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1901097</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1018,7 +1018,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1901098</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1901245</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1902902</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1078,7 +1078,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1905037</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1092,13 +1092,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1990316</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:1990462</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1138,7 +1138,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>&lt;built-in function id&gt;</t>
+          <t>GO:2000785</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">

</xml_diff>